<commit_message>
Worked on Excel Data Analysis Exercises
</commit_message>
<xml_diff>
--- a/LinkedIn/Excel_Data_Analysis/Exercise Files/Chapter02/Forecast.xlsx
+++ b/LinkedIn/Excel_Data_Analysis/Exercise Files/Chapter02/Forecast.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Curtis\Desktop\Exercise Files\Chapter02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtalebiz\Desktop\Jupyter\Examples\LinkedIn\Excel_Data_Analysis\Exercise Files\Chapter02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DF5721-8F3D-485C-BDB0-4F8FE1F45092}" xr6:coauthVersionLast="39" xr6:coauthVersionMax="39" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB349BC-156E-4564-A009-059EA502724E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trend" sheetId="1" r:id="rId1"/>
     <sheet name="Forecast" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -436,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,20 +527,32 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
+      <c r="B10" s="2">
+        <v>412750</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
+      <c r="B11" s="2">
+        <v>426333.33333333302</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
+      <c r="B12" s="2">
+        <v>439916.66666666599</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
+      </c>
+      <c r="B13" s="2">
+        <v>453500</v>
       </c>
     </row>
   </sheetData>
@@ -546,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +597,13 @@
       <c r="B2" s="1">
         <v>35</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="D2">
+        <v>110</v>
+      </c>
+      <c r="E2" s="1">
+        <f>_xlfn.FORECAST.LINEAR(D2, B2:B27, A2:A27)</f>
+        <v>146.57832321175144</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">

</xml_diff>